<commit_message>
18/07/2025 Creación de Modelos
</commit_message>
<xml_diff>
--- a/docs/GANTT.xlsx
+++ b/docs/GANTT.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28129"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DA4BD561-3A1A-4A3E-AB1D-2CCE4DCCB7D1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CFC63EFD-9999-4D11-90B2-91DCE667510E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -2384,7 +2384,7 @@
   <dimension ref="A1:CG70"/>
   <sheetViews>
     <sheetView showGridLines="0" showRowColHeaders="0" tabSelected="1" showRuler="0" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="70" workbookViewId="0">
-      <pane xSplit="8" ySplit="8" topLeftCell="I9" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="8" ySplit="8" topLeftCell="I25" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="I1" sqref="I1"/>
       <selection pane="bottomLeft" activeCell="A9" sqref="A9"/>
       <selection pane="bottomRight" activeCell="D8" sqref="D8"/>

</xml_diff>